<commit_message>
Muestra por pantalla fallos en Email y nombre después de la lectura. Falta pulirlo
</commit_message>
<xml_diff>
--- a/src/test/resources/testCheck.xlsx
+++ b/src/test/resources/testCheck.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Nombre</t>
   </si>
@@ -44,9 +44,6 @@
   </si>
   <si>
     <t>53678541Z</t>
-  </si>
-  <si>
-    <t>Jorge Riopedre Vega</t>
   </si>
   <si>
     <t>48976526C</t>
@@ -379,7 +376,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -390,7 +387,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,7 +418,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2">
         <v>350</v>
@@ -435,21 +432,18 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3">
         <v>440</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4">
         <v>220</v>

</xml_diff>